<commit_message>
Quickfix mistake in C matric for HCFC123 and 124.
</commit_message>
<xml_diff>
--- a/Data/NPRI_IW_concordance.xlsx
+++ b/Data/NPRI_IW_concordance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\PycharmProjects\OpenIOCanada\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F7A13D-3BEA-42F8-80E2-4F1678F782F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DA931E-6E6E-4F18-ADDD-A01BABF894D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -555,15 +555,9 @@
     <t>HCFC-123 (all isomers)</t>
   </si>
   <si>
-    <t>Ethane, 2-chloro-1,1,1,2-tetrafluoro-, HCFC-124</t>
-  </si>
-  <si>
     <t>HCFC-124 (all isomers)</t>
   </si>
   <si>
-    <t>Ethane, 2,2-dichloro-1,1,1-trifluoro-, HCFC-123</t>
-  </si>
-  <si>
     <t>HCFC-142b</t>
   </si>
   <si>
@@ -1399,6 +1393,12 @@
   </si>
   <si>
     <t>1-Pentene</t>
+  </si>
+  <si>
+    <t>Ethane, 2-chloro-1,1,1,2-tetrafluoro-, HCFC-123</t>
+  </si>
+  <si>
+    <t>Ethane, 2,2-dichloro-1,1,1-trifluoro-, HCFC-124</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="E291" sqref="E291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2684,556 +2684,556 @@
         <v>175</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>176</v>
+        <v>456</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>178</v>
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B126" s="4"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B127" s="4"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B128" s="4"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B130" s="4"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B134" s="4"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B135" s="4"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B136" s="4"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B137" s="4"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B139" s="4"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B140" s="4"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B142" s="4"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B147" s="4"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B148" s="4"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B158" s="4"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B159" s="4"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B165" s="4"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B171" s="4"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B173" s="4"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B174" s="4"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B175" s="4"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B177" s="4"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B183" s="4"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B186" s="4"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B187" s="4"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B194" s="4"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B195" s="4"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B196" s="4"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B197" s="4"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>8</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>10</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>14</v>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>25</v>
@@ -3265,13 +3265,13 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B202" s="4"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>44</v>
@@ -3279,15 +3279,15 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>57</v>
@@ -3295,13 +3295,13 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B206" s="4"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>66</v>
@@ -3309,19 +3309,19 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B208" s="4"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B209" s="4"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B210" s="4" t="s">
         <v>112</v>
@@ -3329,45 +3329,45 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B211" s="4"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B212" s="4"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B213" s="4"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B214" s="4"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B216" s="4"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>150</v>
@@ -3375,33 +3375,33 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B218" s="4"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B219" s="4"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B221" s="4"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>158</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>159</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>164</v>
@@ -3425,7 +3425,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>167</v>
@@ -3433,15 +3433,15 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B227" s="4" t="s">
         <v>172</v>
@@ -3449,730 +3449,730 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B229" s="4"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B230" s="4"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B231" s="4"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B232" s="4"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B234" s="4"/>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B235" s="4"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B237" s="4"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B241" s="4"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B242" s="4"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B243" s="4"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B244" s="4"/>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B245" s="4"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B246" s="4"/>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B247" s="4"/>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B248" s="4"/>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B249" s="4"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B252" s="4"/>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B253" s="4"/>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B254" s="4"/>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B255" s="4"/>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B256" s="4"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B258" s="4"/>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B262" s="4"/>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B263" s="4"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B265" s="4"/>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B268" s="4"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B269" s="4"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B273" s="4"/>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B282" s="4"/>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B285" s="4"/>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B288" s="4"/>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B296" s="4"/>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" s="3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" s="3" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" s="3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="3" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" s="3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" s="3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Function to extract self/Y with disaggregated sectors created.
</commit_message>
<xml_diff>
--- a/Data/NPRI_IW_concordance.xlsx
+++ b/Data/NPRI_IW_concordance.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\PycharmProjects\OpenIOCanada\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F55FBE-99AD-4D06-95AA-595CB7820B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A5CCEA-92D5-46CE-A035-2B37568321B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2017" sheetId="1" r:id="rId1"/>
-    <sheet name="2018" sheetId="2" r:id="rId2"/>
+    <sheet name="2014" sheetId="5" r:id="rId1"/>
+    <sheet name="2015" sheetId="4" r:id="rId2"/>
+    <sheet name="2016" sheetId="3" r:id="rId3"/>
+    <sheet name="2017" sheetId="1" r:id="rId4"/>
+    <sheet name="2018" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1907,11 +1910,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB55BFBF-5584-48E4-B5FE-7830A527B831}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29B4954-BC35-4C45-9940-3EFBFABB77B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146099DD-6949-4CCC-9C1A-62A51C5DE123}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B326"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4337,11 +4380,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DCAA807-66A6-479E-901F-554D2A7707A7}">
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>